<commit_message>
Prueba Login Google y Facebook
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -247,12 +247,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="8032397"/>
-        <c:axId val="11328637"/>
-        <c:axId val="6350490"/>
+        <c:axId val="6273774"/>
+        <c:axId val="5127696"/>
+        <c:axId val="11784987"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="8032397"/>
+        <c:axId val="6273774"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +279,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11328637"/>
+        <c:crossAx val="5127696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +288,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11328637"/>
+        <c:axId val="5127696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -309,12 +309,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8032397"/>
+        <c:crossAx val="6273774"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="6350490"/>
+        <c:axId val="11784987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,7 +335,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11328637"/>
+        <c:crossAx val="5127696"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -474,12 +474,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="7787474"/>
-        <c:axId val="9634072"/>
-        <c:axId val="13747308"/>
+        <c:axId val="15664119"/>
+        <c:axId val="8431262"/>
+        <c:axId val="16569565"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="7787474"/>
+        <c:axId val="15664119"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +506,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9634072"/>
+        <c:crossAx val="8431262"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,7 +515,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9634072"/>
+        <c:axId val="8431262"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,12 +536,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7787474"/>
+        <c:crossAx val="15664119"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="13747308"/>
+        <c:axId val="16569565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +562,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9634072"/>
+        <c:crossAx val="8431262"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>

</xml_diff>

<commit_message>
Se implemento el scrollbar para los graficos de todas las redes sociales
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -187,23 +187,65 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Blog'!$B$6:$B$6</c:f>
+              <c:f>'Blog'!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>01 Jan - 31 Jan</c:v>
+                  <c:v>01 Oct - 16 Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17 Oct - 31 Oct</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01 Nov - 15 Nov</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16 Nov - 30 Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>01 Dec - 03 Dec</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>04 Dec - 10 Dec</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11 Dec - 15 Dec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16 Dec - 20 Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Blog'!$B$8:$B$8</c:f>
+              <c:f>'Blog'!$B$8:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -225,34 +267,76 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Blog'!$B$6:$B$6</c:f>
+              <c:f>'Blog'!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>01 Jan - 31 Jan</c:v>
+                  <c:v>01 Oct - 16 Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17 Oct - 31 Oct</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01 Nov - 15 Nov</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16 Nov - 30 Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>01 Dec - 03 Dec</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>04 Dec - 10 Dec</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11 Dec - 15 Dec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16 Dec - 20 Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Blog'!$B$10:$B$10</c:f>
+              <c:f>'Blog'!$B$10:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="6273774"/>
-        <c:axId val="5127696"/>
-        <c:axId val="11784987"/>
+        <c:axId val="3349563"/>
+        <c:axId val="13654679"/>
+        <c:axId val="13327745"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="6273774"/>
+        <c:axId val="3349563"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +363,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5127696"/>
+        <c:crossAx val="13654679"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +372,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5127696"/>
+        <c:axId val="13654679"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -309,12 +393,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6273774"/>
+        <c:crossAx val="3349563"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="11784987"/>
+        <c:axId val="13327745"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,7 +419,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5127696"/>
+        <c:crossAx val="13654679"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -414,23 +498,65 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Blog'!$B$6:$B$6</c:f>
+              <c:f>'Blog'!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>01 Jan - 31 Jan</c:v>
+                  <c:v>01 Oct - 16 Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17 Oct - 31 Oct</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01 Nov - 15 Nov</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16 Nov - 30 Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>01 Dec - 03 Dec</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>04 Dec - 10 Dec</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11 Dec - 15 Dec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16 Dec - 20 Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Blog'!$B$13:$B$13</c:f>
+              <c:f>'Blog'!$B$13:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>879.0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>856.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,34 +578,76 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Blog'!$B$6:$B$6</c:f>
+              <c:f>'Blog'!$B$6:$I$6</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>01 Jan - 31 Jan</c:v>
+                  <c:v>01 Oct - 16 Oct</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17 Oct - 31 Oct</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01 Nov - 15 Nov</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16 Nov - 30 Nov</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>01 Dec - 03 Dec</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>04 Dec - 10 Dec</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11 Dec - 15 Dec</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16 Dec - 20 Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Blog'!$B$14:$B$14</c:f>
+              <c:f>'Blog'!$B$14:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>475.0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>567.0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15664119"/>
-        <c:axId val="8431262"/>
-        <c:axId val="16569565"/>
+        <c:axId val="1973223"/>
+        <c:axId val="7209378"/>
+        <c:axId val="361906"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="15664119"/>
+        <c:axId val="1973223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +674,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8431262"/>
+        <c:crossAx val="7209378"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,7 +683,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8431262"/>
+        <c:axId val="7209378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,12 +704,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15664119"/>
+        <c:crossAx val="1973223"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="16569565"/>
+        <c:axId val="361906"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +730,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8431262"/>
+        <c:crossAx val="7209378"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -647,6 +815,105 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -660,8 +927,15 @@
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.898876404494384"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.998876404494382"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="14"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -683,7 +957,42 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>01 Jan - 31 Jan</t>
+          <t>01 Oct - 16 Oct</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>17 Oct - 31 Oct</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>01 Nov - 15 Nov</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>16 Nov - 30 Nov</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>01 Dec - 03 Dec</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr">
+        <is>
+          <t>04 Dec - 10 Dec</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>11 Dec - 15 Dec</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>16 Dec - 20 Dec</t>
         </is>
       </c>
     </row>
@@ -694,6 +1003,13 @@
         </is>
       </c>
       <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" customHeight="1" ht="20">
       <c r="A8" s="6" t="inlineStr">
@@ -704,6 +1020,27 @@
       <c r="B8" s="6">
         <v>1</v>
       </c>
+      <c r="C8" s="6">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6">
+        <v>90</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45</v>
+      </c>
+      <c r="H8" s="6">
+        <v>45</v>
+      </c>
+      <c r="I8" s="6">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" customHeight="1" ht="20">
       <c r="A9" s="6" t="inlineStr">
@@ -714,6 +1051,27 @@
       <c r="B9" s="6">
         <v>0.0</v>
       </c>
+      <c r="C9" s="6">
+        <v>400.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>80.0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>900.0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>-50.0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="10" customHeight="1" ht="20">
       <c r="A10" s="6" t="inlineStr">
@@ -724,6 +1082,27 @@
       <c r="B10" s="6">
         <v>2</v>
       </c>
+      <c r="C10" s="6">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6">
+        <v>46</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6">
+        <v>67</v>
+      </c>
+      <c r="H10" s="6">
+        <v>567</v>
+      </c>
+      <c r="I10" s="6">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" customHeight="1" ht="20">
       <c r="A11" s="6" t="inlineStr">
@@ -734,6 +1113,27 @@
       <c r="B11" s="6">
         <v>0.0</v>
       </c>
+      <c r="C11" s="6">
+        <v>200.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>33.33</v>
+      </c>
+      <c r="E11" s="6">
+        <v>475.0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-82.61</v>
+      </c>
+      <c r="G11" s="6">
+        <v>737.5</v>
+      </c>
+      <c r="H11" s="6">
+        <v>746.27</v>
+      </c>
+      <c r="I11" s="6">
+        <v>-86.6</v>
+      </c>
     </row>
     <row r="12" customHeight="1" ht="20">
       <c r="A12" s="4" t="inlineStr">
@@ -742,6 +1142,13 @@
         </is>
       </c>
       <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" customHeight="1" ht="20">
       <c r="A13" s="6" t="inlineStr">
@@ -752,6 +1159,27 @@
       <c r="B13" s="6">
         <v>3.0</v>
       </c>
+      <c r="C13" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>7.0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>87.0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>56.0</v>
+      </c>
+      <c r="G13" s="6">
+        <v>879.0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>9.0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>856.0</v>
+      </c>
     </row>
     <row r="14" customHeight="1" ht="20">
       <c r="A14" s="6" t="inlineStr">
@@ -762,6 +1190,27 @@
       <c r="B14" s="6">
         <v>4.0</v>
       </c>
+      <c r="C14" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6.0</v>
+      </c>
+      <c r="E14" s="6">
+        <v>35.0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>475.0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>98.0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>567.0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>35.0</v>
+      </c>
     </row>
     <row r="15" customHeight="1" ht="20">
       <c r="A15" s="6" t="inlineStr">
@@ -771,6 +1220,27 @@
       </c>
       <c r="B15" s="6">
         <v>5</v>
+      </c>
+      <c r="C15" s="6">
+        <v>9</v>
+      </c>
+      <c r="D15" s="6">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6">
+        <v>90</v>
+      </c>
+      <c r="F15" s="6">
+        <v>798</v>
+      </c>
+      <c r="G15" s="6">
+        <v>567</v>
+      </c>
+      <c r="H15" s="6">
+        <v>476</v>
+      </c>
+      <c r="I15" s="6">
+        <v>98</v>
       </c>
     </row>
     <row r="16"/>
@@ -837,6 +1307,111 @@
     <row r="71"/>
     <row r="72"/>
     <row r="73"/>
+    <row r="74">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>Titulo 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t>Imagen de Prueba 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132">
+      <c r="A132" s="3" t="inlineStr">
+        <is>
+          <t>Titulo 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>

</xml_diff>

<commit_message>
Se implemento Reporte para Flickr
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Facebook" sheetId="1" r:id="rId1"/>
     <sheet name="Blog" sheetId="2" r:id="rId2"/>
+    <sheet name="Flickr" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -15,7 +16,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -67,8 +68,31 @@
       <sz val="11"/>
       <family val="1"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,8 +119,18 @@
         <fgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border/>
     <border>
       <left style="thin">
@@ -196,11 +230,53 @@
         <color rgb="#00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -213,6 +289,11 @@
     <xf borderId="5" numFmtId="0" fontId="6" fillId="4" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="6" numFmtId="0" fontId="7" fillId="5" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="7" numFmtId="0" fontId="8" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="9" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="8" numFmtId="0" fontId="10" fillId="6" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="9" numFmtId="0" fontId="11" fillId="7" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="10" numFmtId="0" fontId="12" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
@@ -413,12 +494,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="12410912"/>
-        <c:axId val="10235619"/>
-        <c:axId val="14088470"/>
+        <c:axId val="14829237"/>
+        <c:axId val="10455957"/>
+        <c:axId val="14255773"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="12410912"/>
+        <c:axId val="14829237"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +526,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10235619"/>
+        <c:crossAx val="10455957"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -454,7 +535,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10235619"/>
+        <c:axId val="10455957"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,12 +556,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12410912"/>
+        <c:crossAx val="14829237"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="14088470"/>
+        <c:axId val="14255773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +582,246 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10235619"/>
+        <c:crossAx val="10455957"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Inversion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>-9781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inversion Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$18:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>11352.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>20574.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="979272"/>
+        <c:axId val="4068479"/>
+        <c:axId val="2087439"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="979272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4068479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="4068479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="979272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="2087439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4068479"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -714,12 +1034,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="6312156"/>
-        <c:axId val="3953609"/>
-        <c:axId val="5053514"/>
+        <c:axId val="11952602"/>
+        <c:axId val="15031624"/>
+        <c:axId val="9719783"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="6312156"/>
+        <c:axId val="11952602"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +1066,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3953609"/>
+        <c:crossAx val="15031624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -755,7 +1075,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3953609"/>
+        <c:axId val="15031624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,12 +1096,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6312156"/>
+        <c:crossAx val="11952602"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="5053514"/>
+        <c:axId val="9719783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +1122,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3953609"/>
+        <c:crossAx val="15031624"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1015,12 +1335,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1948283"/>
-        <c:axId val="6876761"/>
-        <c:axId val="12697077"/>
+        <c:axId val="754670"/>
+        <c:axId val="7988881"/>
+        <c:axId val="1043027"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="1948283"/>
+        <c:axId val="754670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1367,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6876761"/>
+        <c:crossAx val="7988881"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1056,7 +1376,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6876761"/>
+        <c:axId val="7988881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,12 +1397,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1948283"/>
+        <c:crossAx val="754670"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="12697077"/>
+        <c:axId val="1043027"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1423,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6876761"/>
+        <c:crossAx val="7988881"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1266,12 +1586,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1957976"/>
-        <c:axId val="186574"/>
-        <c:axId val="6340167"/>
+        <c:axId val="2182506"/>
+        <c:axId val="11235310"/>
+        <c:axId val="13918763"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="1957976"/>
+        <c:axId val="2182506"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1298,7 +1618,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186574"/>
+        <c:crossAx val="11235310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1307,7 +1627,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186574"/>
+        <c:axId val="11235310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,12 +1648,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1957976"/>
+        <c:crossAx val="2182506"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="6340167"/>
+        <c:axId val="13918763"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1354,7 +1674,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186574"/>
+        <c:crossAx val="11235310"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1717,12 +2037,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="11450406"/>
-        <c:axId val="7207534"/>
-        <c:axId val="6017680"/>
+        <c:axId val="15573726"/>
+        <c:axId val="7412841"/>
+        <c:axId val="13983815"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="11450406"/>
+        <c:axId val="15573726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1749,7 +2069,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7207534"/>
+        <c:crossAx val="7412841"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1758,7 +2078,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7207534"/>
+        <c:axId val="7412841"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,12 +2099,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11450406"/>
+        <c:crossAx val="15573726"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="6017680"/>
+        <c:axId val="13983815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1805,7 +2125,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7207534"/>
+        <c:crossAx val="7412841"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2028,12 +2348,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="7499822"/>
-        <c:axId val="4673402"/>
-        <c:axId val="6043899"/>
+        <c:axId val="9967974"/>
+        <c:axId val="4940504"/>
+        <c:axId val="1353257"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="7499822"/>
+        <c:axId val="9967974"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2380,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4673402"/>
+        <c:crossAx val="4940504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2069,7 +2389,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4673402"/>
+        <c:axId val="4940504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2090,12 +2410,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7499822"/>
+        <c:crossAx val="9967974"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="6043899"/>
+        <c:axId val="1353257"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,7 +2436,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4673402"/>
+        <c:crossAx val="4940504"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2339,12 +2659,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="3644818"/>
-        <c:axId val="2044325"/>
-        <c:axId val="5768662"/>
+        <c:axId val="15766561"/>
+        <c:axId val="6053178"/>
+        <c:axId val="2025251"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="3644818"/>
+        <c:axId val="15766561"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2371,7 +2691,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2044325"/>
+        <c:crossAx val="6053178"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2380,7 +2700,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2044325"/>
+        <c:axId val="6053178"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2401,12 +2721,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3644818"/>
+        <c:crossAx val="15766561"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="5768662"/>
+        <c:axId val="2025251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,7 +2747,529 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2044325"/>
+        <c:crossAx val="6053178"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Comunidad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>-9781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>9876</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="10889920"/>
+        <c:axId val="8327261"/>
+        <c:axId val="8635189"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="10889920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8327261"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="8327261"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10889920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="8635189"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8327261"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Interactividad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Visitas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>978</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Comentarios</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$12:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Favorios</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Flickr'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Flickr'!$C$13:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="9087109"/>
+        <c:axId val="5361159"/>
+        <c:axId val="12121698"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="9087109"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="5361159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="5361159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9087109"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="12121698"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="5361159"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2835,6 +3677,167 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="item_2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="item_2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="item_2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
@@ -4895,4 +5898,665 @@
   <pageSetup orientation="landscape" paperSize="9"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA200"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.8988764044943816"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.68988764044944"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>PAGINA DE BLOG</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6" customHeight="1" ht="20">
+      <c r="A6" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B6" s="15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C6" s="15" t="inlineStr">
+        <is>
+          <t>01 Nov - 01 Nov</t>
+        </is>
+      </c>
+      <c r="D6" s="15" t="inlineStr">
+        <is>
+          <t>02 Nov - 02 Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" customHeight="1" ht="20">
+      <c r="A7" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B7" s="14" t="inlineStr">
+        <is>
+          <t>Comunidad</t>
+        </is>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" customHeight="1" ht="20">
+      <c r="A8" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B8" s="16" t="inlineStr">
+        <is>
+          <t># nuevos contactos</t>
+        </is>
+      </c>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16">
+        <v>-9781</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" ht="20">
+      <c r="A9" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B9" s="16" t="inlineStr">
+        <is>
+          <t># contactos</t>
+        </is>
+      </c>
+      <c r="C9" s="16">
+        <v>9876</v>
+      </c>
+      <c r="D9" s="16">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" ht="20">
+      <c r="A10" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B10" s="14" t="inlineStr">
+        <is>
+          <t>Interactividad</t>
+        </is>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" customHeight="1" ht="20">
+      <c r="A11" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B11" s="16" t="inlineStr">
+        <is>
+          <t># Visitas</t>
+        </is>
+      </c>
+      <c r="C11" s="16">
+        <v>978</v>
+      </c>
+      <c r="D11" s="16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" ht="20">
+      <c r="A12" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B12" s="16" t="inlineStr">
+        <is>
+          <t># Comentarios</t>
+        </is>
+      </c>
+      <c r="C12" s="16">
+        <v>768</v>
+      </c>
+      <c r="D12" s="16">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" ht="20">
+      <c r="A13" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B13" s="16" t="inlineStr">
+        <is>
+          <t># Favoritos</t>
+        </is>
+      </c>
+      <c r="C13" s="16">
+        <v>768</v>
+      </c>
+      <c r="D13" s="16">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" ht="20">
+      <c r="A14" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B14" s="14" t="inlineStr">
+        <is>
+          <t>Inversion</t>
+        </is>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" customHeight="1" ht="20">
+      <c r="A15" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B15" s="16" t="inlineStr">
+        <is>
+          <t>Inversion Agencia</t>
+        </is>
+      </c>
+      <c r="C15" s="16">
+        <v>978.0</v>
+      </c>
+      <c r="D15" s="16">
+        <v>6798.0</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" ht="20">
+      <c r="A16" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B16" s="16" t="inlineStr">
+        <is>
+          <t>Inversion nuevas acciones</t>
+        </is>
+      </c>
+      <c r="C16" s="16">
+        <v>687.0</v>
+      </c>
+      <c r="D16" s="16">
+        <v>6987.0</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" ht="20">
+      <c r="A17" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>Inversion anuncios</t>
+        </is>
+      </c>
+      <c r="C17" s="16">
+        <v>9687.0</v>
+      </c>
+      <c r="D17" s="16">
+        <v>6789.0</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" ht="20">
+      <c r="A18" s="17" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B18" s="16" t="inlineStr">
+        <is>
+          <t>Inversion Total</t>
+        </is>
+      </c>
+      <c r="C18" s="16">
+        <v>11352.0</v>
+      </c>
+      <c r="D18" s="16">
+        <v>20574.0</v>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>Comentario para la Tabla de Flickr</t>
+        </is>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>GRAFICOS BLOG</t>
+        </is>
+      </c>
+    </row>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="66"/>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Comunidad Flickr</t>
+        </is>
+      </c>
+    </row>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105">
+      <c r="A105" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="106"/>
+    <row r="107">
+      <c r="A107" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B107" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Interacciones Flickr</t>
+        </is>
+      </c>
+    </row>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147">
+      <c r="A147" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B147" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="148"/>
+    <row r="149">
+      <c r="A149" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B149" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Inversion Flickr</t>
+        </is>
+      </c>
+    </row>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164">
+      <c r="A164" s="13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B164" s="13" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Flickr 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191">
+      <c r="A191" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B191" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="192"/>
+    <row r="193">
+      <c r="A193" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B193" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba Flickr 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206">
+      <c r="A206" s="13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B206" s="13" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Flickr 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233">
+      <c r="A233" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B233" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="234"/>
+    <row r="235">
+      <c r="A235" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B235" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba Flickr 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0" left="0" bottom="0" top="0" footer="0.5" header="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se implemento Reporte para Google+
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -6,6 +6,8 @@
     <sheet name="Facebook" sheetId="1" r:id="rId1"/>
     <sheet name="Blog" sheetId="2" r:id="rId2"/>
     <sheet name="Flickr" sheetId="3" r:id="rId3"/>
+    <sheet name="Foursquare" sheetId="4" r:id="rId4"/>
+    <sheet name="Google+" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -16,7 +18,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="21">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -91,8 +93,54 @@
       <sz val="11"/>
       <family val="1"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +177,28 @@
         <fgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border/>
     <border>
       <left style="thin">
@@ -272,11 +340,95 @@
         <color rgb="#00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#00000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -294,6 +446,16 @@
     <xf borderId="8" numFmtId="0" fontId="10" fillId="6" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="9" numFmtId="0" fontId="11" fillId="7" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="10" numFmtId="0" fontId="12" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="13" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="11" numFmtId="0" fontId="14" fillId="8" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="12" numFmtId="0" fontId="15" fillId="9" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="13" numFmtId="0" fontId="16" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="17" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="14" numFmtId="0" fontId="18" fillId="10" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="15" numFmtId="0" fontId="19" fillId="11" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="16" numFmtId="0" fontId="20" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
@@ -494,12 +656,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="14829237"/>
-        <c:axId val="10455957"/>
-        <c:axId val="14255773"/>
+        <c:axId val="3053057"/>
+        <c:axId val="13948330"/>
+        <c:axId val="14921799"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="14829237"/>
+        <c:axId val="3053057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +688,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10455957"/>
+        <c:crossAx val="13948330"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -535,7 +697,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10455957"/>
+        <c:axId val="13948330"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,12 +718,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14829237"/>
+        <c:crossAx val="3053057"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="14255773"/>
+        <c:axId val="14921799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +744,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10455957"/>
+        <c:crossAx val="13948330"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -733,12 +895,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="979272"/>
-        <c:axId val="4068479"/>
-        <c:axId val="2087439"/>
+        <c:axId val="2762234"/>
+        <c:axId val="10368096"/>
+        <c:axId val="332068"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="979272"/>
+        <c:axId val="2762234"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,7 +927,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4068479"/>
+        <c:crossAx val="10368096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +936,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4068479"/>
+        <c:axId val="10368096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -795,12 +957,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="979272"/>
+        <c:crossAx val="2762234"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2087439"/>
+        <c:axId val="332068"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +983,1246 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4068479"/>
+        <c:crossAx val="10368096"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Followers</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos followers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Foursquare'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Foursquare'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>260</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># followers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Foursquare'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Foursquare'!$C$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="3502585"/>
+        <c:axId val="14589514"/>
+        <c:axId val="4067764"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="3502585"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14589514"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="14589514"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="3502585"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="4067764"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14589514"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Ofertas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># unlocks  total de ofertas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Foursquare'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Foursquare'!$C$10:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># visitas total de las ofertas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Foursquare'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Foursquare'!$C$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>789</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="10880192"/>
+        <c:axId val="7792959"/>
+        <c:axId val="4559485"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="10880192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7792959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7792959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10880192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="4559485"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7792959"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Comunidad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>769</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="3148857"/>
+        <c:axId val="1440246"/>
+        <c:axId val="12421718"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="3148857"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1440246"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1440246"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="3148857"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="12421718"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1440246"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Interactividad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(+1s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$12:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Compartir Contenido</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$13:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>9876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Interacciones</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$14:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>894</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>10854</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="8101185"/>
+        <c:axId val="11727768"/>
+        <c:axId val="5541768"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="8101185"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11727768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11727768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8101185"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="5541768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11727768"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Inversion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos contactos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inversion Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Google+'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Google+'!$C$20:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>14385.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>20421.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="6186273"/>
+        <c:axId val="4419120"/>
+        <c:axId val="12414217"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="6186273"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4419120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="4419120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6186273"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="12414217"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4419120"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1034,12 +2435,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="11952602"/>
-        <c:axId val="15031624"/>
-        <c:axId val="9719783"/>
+        <c:axId val="9749568"/>
+        <c:axId val="13254927"/>
+        <c:axId val="1246064"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="11952602"/>
+        <c:axId val="9749568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1066,7 +2467,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15031624"/>
+        <c:crossAx val="13254927"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1075,7 +2476,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15031624"/>
+        <c:axId val="13254927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,12 +2497,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11952602"/>
+        <c:crossAx val="9749568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="9719783"/>
+        <c:axId val="1246064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +2523,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15031624"/>
+        <c:crossAx val="13254927"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1335,12 +2736,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="754670"/>
-        <c:axId val="7988881"/>
-        <c:axId val="1043027"/>
+        <c:axId val="7375766"/>
+        <c:axId val="11882248"/>
+        <c:axId val="10108274"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="754670"/>
+        <c:axId val="7375766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +2768,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7988881"/>
+        <c:crossAx val="11882248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1376,7 +2777,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7988881"/>
+        <c:axId val="11882248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1397,12 +2798,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="754670"/>
+        <c:crossAx val="7375766"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="1043027"/>
+        <c:axId val="10108274"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +2824,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7988881"/>
+        <c:crossAx val="11882248"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1586,12 +2987,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2182506"/>
-        <c:axId val="11235310"/>
-        <c:axId val="13918763"/>
+        <c:axId val="11938197"/>
+        <c:axId val="13557172"/>
+        <c:axId val="10501050"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="2182506"/>
+        <c:axId val="11938197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +3019,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11235310"/>
+        <c:crossAx val="13557172"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1627,7 +3028,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11235310"/>
+        <c:axId val="13557172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,12 +3049,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2182506"/>
+        <c:crossAx val="11938197"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="13918763"/>
+        <c:axId val="10501050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +3075,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11235310"/>
+        <c:crossAx val="13557172"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2037,12 +3438,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15573726"/>
-        <c:axId val="7412841"/>
-        <c:axId val="13983815"/>
+        <c:axId val="11803452"/>
+        <c:axId val="16055833"/>
+        <c:axId val="62209"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="15573726"/>
+        <c:axId val="11803452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +3470,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7412841"/>
+        <c:crossAx val="16055833"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2078,7 +3479,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7412841"/>
+        <c:axId val="16055833"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,12 +3500,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15573726"/>
+        <c:crossAx val="11803452"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="13983815"/>
+        <c:axId val="62209"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +3526,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7412841"/>
+        <c:crossAx val="16055833"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2348,12 +3749,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="9967974"/>
-        <c:axId val="4940504"/>
-        <c:axId val="1353257"/>
+        <c:axId val="6644333"/>
+        <c:axId val="12909329"/>
+        <c:axId val="14081562"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="9967974"/>
+        <c:axId val="6644333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2380,7 +3781,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4940504"/>
+        <c:crossAx val="12909329"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2389,7 +3790,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4940504"/>
+        <c:axId val="12909329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2410,12 +3811,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9967974"/>
+        <c:crossAx val="6644333"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="1353257"/>
+        <c:axId val="14081562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2436,7 +3837,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4940504"/>
+        <c:crossAx val="12909329"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2659,12 +4060,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15766561"/>
-        <c:axId val="6053178"/>
-        <c:axId val="2025251"/>
+        <c:axId val="1386807"/>
+        <c:axId val="743170"/>
+        <c:axId val="1933985"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="15766561"/>
+        <c:axId val="1386807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,7 +4092,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6053178"/>
+        <c:crossAx val="743170"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2700,7 +4101,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6053178"/>
+        <c:axId val="743170"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2721,12 +4122,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15766561"/>
+        <c:crossAx val="1386807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2025251"/>
+        <c:axId val="1933985"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,7 +4148,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6053178"/>
+        <c:crossAx val="743170"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2898,12 +4299,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="10889920"/>
-        <c:axId val="8327261"/>
-        <c:axId val="8635189"/>
+        <c:axId val="8074145"/>
+        <c:axId val="3823222"/>
+        <c:axId val="7565917"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="10889920"/>
+        <c:axId val="8074145"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2930,7 +4331,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8327261"/>
+        <c:crossAx val="3823222"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2939,7 +4340,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8327261"/>
+        <c:axId val="3823222"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2960,12 +4361,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10889920"/>
+        <c:crossAx val="8074145"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="8635189"/>
+        <c:axId val="7565917"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2986,7 +4387,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8327261"/>
+        <c:crossAx val="3823222"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3181,12 +4582,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="9087109"/>
-        <c:axId val="5361159"/>
-        <c:axId val="12121698"/>
+        <c:axId val="15380993"/>
+        <c:axId val="12908585"/>
+        <c:axId val="13495168"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="9087109"/>
+        <c:axId val="15380993"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3213,7 +4614,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5361159"/>
+        <c:crossAx val="12908585"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3222,7 +4623,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5361159"/>
+        <c:axId val="12908585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3243,12 +4644,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9087109"/>
+        <c:crossAx val="15380993"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="12121698"/>
+        <c:axId val="13495168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,7 +4670,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5361159"/>
+        <c:crossAx val="12908585"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3838,6 +5239,298 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="item_3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="item_3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="item_4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="item_4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="item_4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
@@ -5926,7 +7619,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>PAGINA DE BLOG</t>
+          <t>PAGINA FLICKR</t>
         </is>
       </c>
     </row>
@@ -6207,7 +7900,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>GRAFICOS BLOG</t>
+          <t>GRAFICOS FLICKR</t>
         </is>
       </c>
     </row>
@@ -6559,4 +8252,1188 @@
   <pageSetup orientation="landscape" paperSize="9"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA200"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.8988764044943816"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.49887640449438"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>PAGINA DE FOURSQUARE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6" customHeight="1" ht="20">
+      <c r="A6" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B6" s="20" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C6" s="20" t="inlineStr">
+        <is>
+          <t>01 Nov - 01 Nov</t>
+        </is>
+      </c>
+      <c r="D6" s="20" t="inlineStr">
+        <is>
+          <t>02 Nov - 02 Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" customHeight="1" ht="20">
+      <c r="A7" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B7" s="19" t="inlineStr">
+        <is>
+          <t>Comunidad</t>
+        </is>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" customHeight="1" ht="20">
+      <c r="A8" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B8" s="21" t="inlineStr">
+        <is>
+          <t># nuevos followers</t>
+        </is>
+      </c>
+      <c r="C8" s="21">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" ht="20">
+      <c r="A9" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B9" s="21" t="inlineStr">
+        <is>
+          <t># followers</t>
+        </is>
+      </c>
+      <c r="C9" s="21">
+        <v>85</v>
+      </c>
+      <c r="D9" s="21">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" ht="20">
+      <c r="A10" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B10" s="21" t="inlineStr">
+        <is>
+          <t># unlocks total de las ofertas</t>
+        </is>
+      </c>
+      <c r="C10" s="21">
+        <v>867</v>
+      </c>
+      <c r="D10" s="21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" ht="20">
+      <c r="A11" s="22" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B11" s="21" t="inlineStr">
+        <is>
+          <t># visitas total de las ofertas</t>
+        </is>
+      </c>
+      <c r="C11" s="21">
+        <v>58</v>
+      </c>
+      <c r="D11" s="21">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="14"/>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Tabla Foursquare</t>
+        </is>
+      </c>
+    </row>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>GRAFICOS FOURSQUARE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="70"/>
+    <row r="71">
+      <c r="A71" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B71" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Followers Foursquare</t>
+        </is>
+      </c>
+    </row>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="110"/>
+    <row r="111">
+      <c r="A111" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B111" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Ofertas Foursquare</t>
+        </is>
+      </c>
+    </row>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126">
+      <c r="A126" s="18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B126" s="18" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Foursquare 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153">
+      <c r="A153" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B153" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="154"/>
+    <row r="155">
+      <c r="A155" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B155" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168">
+      <c r="A168" s="18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B168" s="18" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Foursquare 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195">
+      <c r="A195" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B195" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="196"/>
+    <row r="197">
+      <c r="A197" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B197" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba Foursquare 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0" left="0" bottom="0" top="0" footer="0.5" header="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA200"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.8988764044943816"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="37.39887640449438"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.68988764044944"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>PAGINA DE GOOGLE+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6" customHeight="1" ht="20">
+      <c r="A6" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B6" s="25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C6" s="25" t="inlineStr">
+        <is>
+          <t>01 Nov - 01 Nov</t>
+        </is>
+      </c>
+      <c r="D6" s="25" t="inlineStr">
+        <is>
+          <t>02 Nov - 02 Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" customHeight="1" ht="20">
+      <c r="A7" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B7" s="24" t="inlineStr">
+        <is>
+          <t>Comunidad</t>
+        </is>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" customHeight="1" ht="20">
+      <c r="A8" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B8" s="26" t="inlineStr">
+        <is>
+          <t># nuevos followers</t>
+        </is>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" ht="20">
+      <c r="A9" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B9" s="26" t="inlineStr">
+        <is>
+          <t># followers</t>
+        </is>
+      </c>
+      <c r="C9" s="26">
+        <v>76</v>
+      </c>
+      <c r="D9" s="26">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" ht="20">
+      <c r="A10" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B10" s="26" t="inlineStr">
+        <is>
+          <t>% crecimiento seguidores</t>
+        </is>
+      </c>
+      <c r="C10" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="26">
+        <v>911.842</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" ht="20">
+      <c r="A11" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B11" s="24" t="inlineStr">
+        <is>
+          <t>Interactividad</t>
+        </is>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" customHeight="1" ht="20">
+      <c r="A12" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B12" s="26" t="inlineStr">
+        <is>
+          <t>(+1s)</t>
+        </is>
+      </c>
+      <c r="C12" s="26">
+        <v>96</v>
+      </c>
+      <c r="D12" s="26">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" ht="20">
+      <c r="A13" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B13" s="26" t="inlineStr">
+        <is>
+          <t>Compartir contenido</t>
+        </is>
+      </c>
+      <c r="C13" s="26">
+        <v>798</v>
+      </c>
+      <c r="D13" s="26">
+        <v>9876</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" ht="20">
+      <c r="A14" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B14" s="26" t="inlineStr">
+        <is>
+          <t>Total de Interacciones</t>
+        </is>
+      </c>
+      <c r="C14" s="26">
+        <v>894</v>
+      </c>
+      <c r="D14" s="26">
+        <v>10854</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" ht="20">
+      <c r="A15" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B15" s="26" t="inlineStr">
+        <is>
+          <t>% cambio en interacciones</t>
+        </is>
+      </c>
+      <c r="C15" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="D15" s="26">
+        <v>1114.094</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" ht="20">
+      <c r="A16" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B16" s="24" t="inlineStr">
+        <is>
+          <t>Inversion</t>
+        </is>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" customHeight="1" ht="20">
+      <c r="A17" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B17" s="26" t="inlineStr">
+        <is>
+          <t>Inversion Agencia</t>
+        </is>
+      </c>
+      <c r="C17" s="26">
+        <v>6798.0</v>
+      </c>
+      <c r="D17" s="26">
+        <v>9687.0</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" ht="20">
+      <c r="A18" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B18" s="26" t="inlineStr">
+        <is>
+          <t>Inversion nuevas acciones</t>
+        </is>
+      </c>
+      <c r="C18" s="26">
+        <v>798.0</v>
+      </c>
+      <c r="D18" s="26">
+        <v>9867.0</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" ht="20">
+      <c r="A19" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B19" s="26" t="inlineStr">
+        <is>
+          <t>Inversion anuncios</t>
+        </is>
+      </c>
+      <c r="C19" s="26">
+        <v>6789.0</v>
+      </c>
+      <c r="D19" s="26">
+        <v>867.0</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" ht="20">
+      <c r="A20" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B20" s="26" t="inlineStr">
+        <is>
+          <t>Inversion Total</t>
+        </is>
+      </c>
+      <c r="C20" s="26">
+        <v>14385.0</v>
+      </c>
+      <c r="D20" s="26">
+        <v>20421.0</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24">
+      <c r="A24" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B24" s="0" t="inlineStr">
+        <is>
+          <t>Comentario para la Tabla Google+</t>
+        </is>
+      </c>
+    </row>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>GRAFICOS GOOGLE+</t>
+        </is>
+      </c>
+    </row>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64">
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="65"/>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Comunidad Google+</t>
+        </is>
+      </c>
+    </row>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104">
+      <c r="A104" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="105"/>
+    <row r="106">
+      <c r="A106" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B106" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Interacciones Google+</t>
+        </is>
+      </c>
+    </row>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146">
+      <c r="A146" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B146" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="147"/>
+    <row r="148">
+      <c r="A148" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B148" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Inversion Google+</t>
+        </is>
+      </c>
+    </row>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163">
+      <c r="A163" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B163" s="23" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Google+ 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190">
+      <c r="A190" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B190" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="191"/>
+    <row r="192">
+      <c r="A192" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B192" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Con la imagen de Google+</t>
+        </is>
+      </c>
+    </row>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205">
+      <c r="A205" s="23" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B205" s="23" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Google+ 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232">
+      <c r="A232" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B232" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="233"/>
+    <row r="234">
+      <c r="A234" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B234" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba Google+ 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0" left="0" bottom="0" top="0" footer="0.5" header="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se implemento Reporte para Pinterest
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Foursquare" sheetId="4" r:id="rId4"/>
     <sheet name="Google+" sheetId="5" r:id="rId5"/>
     <sheet name="Linkedin" sheetId="6" r:id="rId6"/>
+    <sheet name="Pinterest" sheetId="7" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -19,7 +20,7 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="29">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -163,8 +164,31 @@
       <sz val="11"/>
       <family val="1"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14"/>
+      <family val="1"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="9"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +255,18 @@
         <fgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border/>
     <border>
       <left style="thin">
@@ -500,11 +534,53 @@
         <color rgb="#00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="#00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="#00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="#00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="#00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -537,6 +613,11 @@
     <xf borderId="17" numFmtId="0" fontId="22" fillId="12" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="18" numFmtId="0" fontId="23" fillId="13" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="19" numFmtId="0" fontId="24" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="25" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="20" numFmtId="0" fontId="26" fillId="14" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="21" numFmtId="0" fontId="27" fillId="15" applyNumberFormat="false" applyFill="true" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="22" numFmtId="0" fontId="28" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
@@ -737,12 +818,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="14990304"/>
-        <c:axId val="6024392"/>
-        <c:axId val="1082410"/>
+        <c:axId val="11757730"/>
+        <c:axId val="11382534"/>
+        <c:axId val="1124757"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="14990304"/>
+        <c:axId val="11757730"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,7 +850,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6024392"/>
+        <c:crossAx val="11382534"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -778,7 +859,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6024392"/>
+        <c:axId val="11382534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,12 +880,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14990304"/>
+        <c:crossAx val="11757730"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="1082410"/>
+        <c:axId val="1124757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +906,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6024392"/>
+        <c:crossAx val="11382534"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -976,12 +1057,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="12705442"/>
-        <c:axId val="10201735"/>
-        <c:axId val="11950954"/>
+        <c:axId val="6911752"/>
+        <c:axId val="15429964"/>
+        <c:axId val="5308118"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="12705442"/>
+        <c:axId val="6911752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1089,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10201735"/>
+        <c:crossAx val="15429964"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1017,7 +1098,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10201735"/>
+        <c:axId val="15429964"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,12 +1119,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12705442"/>
+        <c:crossAx val="6911752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="11950954"/>
+        <c:axId val="5308118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1145,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10201735"/>
+        <c:crossAx val="15429964"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1215,12 +1296,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="16503945"/>
-        <c:axId val="16684898"/>
-        <c:axId val="10837144"/>
+        <c:axId val="8659165"/>
+        <c:axId val="6180558"/>
+        <c:axId val="13710710"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="16503945"/>
+        <c:axId val="8659165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1247,7 +1328,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16684898"/>
+        <c:crossAx val="6180558"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1256,7 +1337,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16684898"/>
+        <c:axId val="6180558"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,12 +1358,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16503945"/>
+        <c:crossAx val="8659165"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="10837144"/>
+        <c:axId val="13710710"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1384,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16684898"/>
+        <c:crossAx val="6180558"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1454,12 +1535,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="4139222"/>
-        <c:axId val="13742816"/>
-        <c:axId val="12835059"/>
+        <c:axId val="11400920"/>
+        <c:axId val="1948933"/>
+        <c:axId val="7499258"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="4139222"/>
+        <c:axId val="11400920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1567,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13742816"/>
+        <c:crossAx val="1948933"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1495,7 +1576,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13742816"/>
+        <c:axId val="1948933"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,12 +1597,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4139222"/>
+        <c:crossAx val="11400920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="12835059"/>
+        <c:axId val="7499258"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1542,7 +1623,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13742816"/>
+        <c:crossAx val="1948933"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1693,12 +1774,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="10810450"/>
-        <c:axId val="13357092"/>
-        <c:axId val="2715130"/>
+        <c:axId val="10286499"/>
+        <c:axId val="6471670"/>
+        <c:axId val="3057640"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="10810450"/>
+        <c:axId val="10286499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1806,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13357092"/>
+        <c:crossAx val="6471670"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1734,7 +1815,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13357092"/>
+        <c:axId val="6471670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,12 +1836,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10810450"/>
+        <c:crossAx val="10286499"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2715130"/>
+        <c:axId val="3057640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +1862,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13357092"/>
+        <c:crossAx val="6471670"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1976,12 +2057,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="12408689"/>
-        <c:axId val="15547672"/>
-        <c:axId val="12274845"/>
+        <c:axId val="15059431"/>
+        <c:axId val="6127190"/>
+        <c:axId val="543490"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="12408689"/>
+        <c:axId val="15059431"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2008,7 +2089,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15547672"/>
+        <c:crossAx val="6127190"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2017,7 +2098,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15547672"/>
+        <c:axId val="6127190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2038,12 +2119,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12408689"/>
+        <c:crossAx val="15059431"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="12274845"/>
+        <c:axId val="543490"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2064,7 +2145,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15547672"/>
+        <c:crossAx val="6127190"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2215,12 +2296,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="15836284"/>
-        <c:axId val="55619"/>
-        <c:axId val="1139464"/>
+        <c:axId val="15679521"/>
+        <c:axId val="2667042"/>
+        <c:axId val="5647200"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="15836284"/>
+        <c:axId val="15679521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +2328,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55619"/>
+        <c:crossAx val="2667042"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2256,7 +2337,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55619"/>
+        <c:axId val="2667042"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,12 +2358,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15836284"/>
+        <c:crossAx val="15679521"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="1139464"/>
+        <c:axId val="5647200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2303,7 +2384,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55619"/>
+        <c:crossAx val="2667042"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2526,12 +2607,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="5059540"/>
-        <c:axId val="1822846"/>
-        <c:axId val="13805411"/>
+        <c:axId val="1742678"/>
+        <c:axId val="15959065"/>
+        <c:axId val="2289240"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="5059540"/>
+        <c:axId val="1742678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2639,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1822846"/>
+        <c:crossAx val="15959065"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2567,7 +2648,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1822846"/>
+        <c:axId val="15959065"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,12 +2669,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5059540"/>
+        <c:crossAx val="1742678"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="13805411"/>
+        <c:axId val="2289240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2614,7 +2695,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1822846"/>
+        <c:crossAx val="15959065"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3317,12 +3398,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="14942875"/>
-        <c:axId val="921629"/>
-        <c:axId val="12248955"/>
+        <c:axId val="573925"/>
+        <c:axId val="8315829"/>
+        <c:axId val="3577617"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="14942875"/>
+        <c:axId val="573925"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3349,7 +3430,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="921629"/>
+        <c:crossAx val="8315829"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3358,7 +3439,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="921629"/>
+        <c:axId val="8315829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3379,12 +3460,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14942875"/>
+        <c:crossAx val="573925"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="12248955"/>
+        <c:axId val="3577617"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3405,7 +3486,661 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="921629"/>
+        <c:crossAx val="8315829"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Comunidad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Nuevos Followers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>8689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># Followers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>8765</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># boards</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$10:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># pins</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$11:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>6978</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="6676456"/>
+        <c:axId val="6687606"/>
+        <c:axId val="9672309"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="6676456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6687606"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="6687606"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6676456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="9672309"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6687606"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Interactividad</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># liked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$13:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>6978</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>756</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># repin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$14:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>6798</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># comments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$15:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># community boards</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$16:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>8769</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="15367442"/>
+        <c:axId val="6136765"/>
+        <c:axId val="15051636"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="15367442"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6136765"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="6136765"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15367442"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="15051636"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6136765"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3618,12 +4353,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="7081364"/>
-        <c:axId val="13969760"/>
-        <c:axId val="3487695"/>
+        <c:axId val="8788557"/>
+        <c:axId val="14597788"/>
+        <c:axId val="16710565"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="7081364"/>
+        <c:axId val="8788557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3650,7 +4385,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13969760"/>
+        <c:crossAx val="14597788"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3659,7 +4394,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13969760"/>
+        <c:axId val="14597788"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3680,12 +4415,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7081364"/>
+        <c:crossAx val="8788557"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="3487695"/>
+        <c:axId val="16710565"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3706,7 +4441,246 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13969760"/>
+        <c:crossAx val="14597788"/>
+        <c:crosses val="autoZero"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>Inversion</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rotX val="0"/>
+      <c:rotY val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v># nuevos followers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>8689</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f/>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inversion Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pinterest'!$C$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>01 Nov - 01 Nov</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>02 Nov - 02 Nov</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pinterest'!$C$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>17554.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>738.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="9607250"/>
+        <c:axId val="16074866"/>
+        <c:axId val="15169080"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="9607250"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16074866"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="16074866"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9607250"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="15169080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="true"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16074866"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3919,12 +4893,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="12477109"/>
-        <c:axId val="1128600"/>
-        <c:axId val="13416820"/>
+        <c:axId val="15050374"/>
+        <c:axId val="8673148"/>
+        <c:axId val="14634632"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="12477109"/>
+        <c:axId val="15050374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3951,7 +4925,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1128600"/>
+        <c:crossAx val="8673148"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3960,7 +4934,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1128600"/>
+        <c:axId val="8673148"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3981,12 +4955,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12477109"/>
+        <c:crossAx val="15050374"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="13416820"/>
+        <c:axId val="14634632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,7 +4981,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1128600"/>
+        <c:crossAx val="8673148"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -4170,12 +5144,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="7889345"/>
-        <c:axId val="14428319"/>
-        <c:axId val="3368787"/>
+        <c:axId val="7521995"/>
+        <c:axId val="15122959"/>
+        <c:axId val="10305862"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="7889345"/>
+        <c:axId val="7521995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4202,7 +5176,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14428319"/>
+        <c:crossAx val="15122959"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4211,7 +5185,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14428319"/>
+        <c:axId val="15122959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4232,12 +5206,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7889345"/>
+        <c:crossAx val="7521995"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="3368787"/>
+        <c:axId val="10305862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4258,7 +5232,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14428319"/>
+        <c:crossAx val="15122959"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -4621,12 +5595,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2572852"/>
-        <c:axId val="2064707"/>
-        <c:axId val="373087"/>
+        <c:axId val="10435266"/>
+        <c:axId val="6699900"/>
+        <c:axId val="15553500"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="2572852"/>
+        <c:axId val="10435266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4653,7 +5627,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064707"/>
+        <c:crossAx val="6699900"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4662,7 +5636,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064707"/>
+        <c:axId val="6699900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4683,12 +5657,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2572852"/>
+        <c:crossAx val="10435266"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="373087"/>
+        <c:axId val="15553500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4709,7 +5683,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2064707"/>
+        <c:crossAx val="6699900"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -4932,12 +5906,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="9398512"/>
-        <c:axId val="2432364"/>
-        <c:axId val="9942821"/>
+        <c:axId val="6009625"/>
+        <c:axId val="10741852"/>
+        <c:axId val="719875"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="9398512"/>
+        <c:axId val="6009625"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4964,7 +5938,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2432364"/>
+        <c:crossAx val="10741852"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4973,7 +5947,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2432364"/>
+        <c:axId val="10741852"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4994,12 +5968,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9398512"/>
+        <c:crossAx val="6009625"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="9942821"/>
+        <c:axId val="719875"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5020,7 +5994,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2432364"/>
+        <c:crossAx val="10741852"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -5243,12 +6217,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="8058719"/>
-        <c:axId val="3879156"/>
-        <c:axId val="8760710"/>
+        <c:axId val="13895722"/>
+        <c:axId val="4136757"/>
+        <c:axId val="2217436"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="8058719"/>
+        <c:axId val="13895722"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5275,7 +6249,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3879156"/>
+        <c:crossAx val="4136757"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5284,7 +6258,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3879156"/>
+        <c:axId val="4136757"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5305,12 +6279,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8058719"/>
+        <c:crossAx val="13895722"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="8760710"/>
+        <c:axId val="2217436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5331,7 +6305,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3879156"/>
+        <c:crossAx val="4136757"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -5482,12 +6456,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="10834041"/>
-        <c:axId val="8103056"/>
-        <c:axId val="3057642"/>
+        <c:axId val="16296193"/>
+        <c:axId val="14130823"/>
+        <c:axId val="14110926"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="10834041"/>
+        <c:axId val="16296193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5514,7 +6488,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8103056"/>
+        <c:crossAx val="14130823"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5523,7 +6497,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8103056"/>
+        <c:axId val="14130823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5544,12 +6518,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10834041"/>
+        <c:crossAx val="16296193"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="3057642"/>
+        <c:axId val="14110926"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5570,7 +6544,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8103056"/>
+        <c:crossAx val="14130823"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -5765,12 +6739,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="4043139"/>
-        <c:axId val="8450184"/>
-        <c:axId val="6042507"/>
+        <c:axId val="11940986"/>
+        <c:axId val="669459"/>
+        <c:axId val="5540882"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="4043139"/>
+        <c:axId val="11940986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5797,7 +6771,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8450184"/>
+        <c:crossAx val="669459"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5806,7 +6780,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8450184"/>
+        <c:axId val="669459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5827,12 +6801,12 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4043139"/>
+        <c:crossAx val="11940986"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="6042507"/>
+        <c:axId val="5540882"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5853,7 +6827,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8450184"/>
+        <c:crossAx val="669459"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -6845,6 +7819,167 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="item_6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="item_6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="item_6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3810000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="" descr=""/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2336800" cy="2161540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
@@ -11804,4 +12939,714 @@
   <pageSetup orientation="landscape" paperSize="9"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AA200"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.8988764044943816"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="37.39887640449438"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>PAGINA DE PINTEREST</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6" customHeight="1" ht="20">
+      <c r="A6" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B6" s="35" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C6" s="35" t="inlineStr">
+        <is>
+          <t>01 Nov - 01 Nov</t>
+        </is>
+      </c>
+      <c r="D6" s="35" t="inlineStr">
+        <is>
+          <t>02 Nov - 02 Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" customHeight="1" ht="20">
+      <c r="A7" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B7" s="34" t="inlineStr">
+        <is>
+          <t>Comunidad</t>
+        </is>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" customHeight="1" ht="20">
+      <c r="A8" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B8" s="36" t="inlineStr">
+        <is>
+          <t># Nuevos Followers</t>
+        </is>
+      </c>
+      <c r="C8" s="36">
+        <v>0</v>
+      </c>
+      <c r="D8" s="36">
+        <v>8689</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" ht="20">
+      <c r="A9" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B9" s="36" t="inlineStr">
+        <is>
+          <t># Followers</t>
+        </is>
+      </c>
+      <c r="C9" s="36">
+        <v>76</v>
+      </c>
+      <c r="D9" s="36">
+        <v>8765</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" ht="20">
+      <c r="A10" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B10" s="36" t="inlineStr">
+        <is>
+          <t># boards</t>
+        </is>
+      </c>
+      <c r="C10" s="36">
+        <v>7</v>
+      </c>
+      <c r="D10" s="36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" ht="20">
+      <c r="A11" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B11" s="36" t="inlineStr">
+        <is>
+          <t># pins</t>
+        </is>
+      </c>
+      <c r="C11" s="36">
+        <v>6978</v>
+      </c>
+      <c r="D11" s="36">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" ht="20">
+      <c r="A12" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B12" s="34" t="inlineStr">
+        <is>
+          <t>Interactividad</t>
+        </is>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" customHeight="1" ht="20">
+      <c r="A13" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B13" s="36" t="inlineStr">
+        <is>
+          <t># liked</t>
+        </is>
+      </c>
+      <c r="C13" s="36">
+        <v>6978</v>
+      </c>
+      <c r="D13" s="36">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" ht="20">
+      <c r="A14" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B14" s="36" t="inlineStr">
+        <is>
+          <t># repin</t>
+        </is>
+      </c>
+      <c r="C14" s="36">
+        <v>6798</v>
+      </c>
+      <c r="D14" s="36">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" ht="20">
+      <c r="A15" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B15" s="36" t="inlineStr">
+        <is>
+          <t># comments</t>
+        </is>
+      </c>
+      <c r="C15" s="36">
+        <v>867</v>
+      </c>
+      <c r="D15" s="36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" ht="20">
+      <c r="A16" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B16" s="36" t="inlineStr">
+        <is>
+          <t># community boards</t>
+        </is>
+      </c>
+      <c r="C16" s="36">
+        <v>8769</v>
+      </c>
+      <c r="D16" s="36">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" ht="20">
+      <c r="A17" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B17" s="34" t="inlineStr">
+        <is>
+          <t>Inversion</t>
+        </is>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+    </row>
+    <row r="18" customHeight="1" ht="20">
+      <c r="A18" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B18" s="36" t="inlineStr">
+        <is>
+          <t>Inversion Agencia</t>
+        </is>
+      </c>
+      <c r="C18" s="36">
+        <v>7869.0</v>
+      </c>
+      <c r="D18" s="36">
+        <v>567.0</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" ht="20">
+      <c r="A19" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B19" s="36" t="inlineStr">
+        <is>
+          <t>Inversion nuevas acciones</t>
+        </is>
+      </c>
+      <c r="C19" s="36">
+        <v>7.0</v>
+      </c>
+      <c r="D19" s="36">
+        <v>86.0</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" ht="20">
+      <c r="A20" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B20" s="36" t="inlineStr">
+        <is>
+          <t>Inversion anuncios</t>
+        </is>
+      </c>
+      <c r="C20" s="36">
+        <v>9678.0</v>
+      </c>
+      <c r="D20" s="36">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" ht="20">
+      <c r="A21" s="37" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B21" s="36" t="inlineStr">
+        <is>
+          <t>Inversion Total</t>
+        </is>
+      </c>
+      <c r="C21" s="36">
+        <v>17554.0</v>
+      </c>
+      <c r="D21" s="36">
+        <v>738.0</v>
+      </c>
+    </row>
+    <row r="22"/>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B25" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Tabla Pinterest</t>
+        </is>
+      </c>
+    </row>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>GRAFICOS PINTEREST</t>
+        </is>
+      </c>
+    </row>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63">
+      <c r="A63" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="64"/>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Seguidores</t>
+        </is>
+      </c>
+    </row>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="104"/>
+    <row r="105">
+      <c r="A105" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B105" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Interacciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145">
+      <c r="A145" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B145" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="146"/>
+    <row r="147">
+      <c r="A147" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B147" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Grafico Inversiones</t>
+        </is>
+      </c>
+    </row>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162">
+      <c r="A162" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B162" s="33" t="inlineStr">
+        <is>
+          <t>Imagen de Prueba Pinterest 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189">
+      <c r="A189" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B189" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="190"/>
+    <row r="191">
+      <c r="A191" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B191" s="0" t="inlineStr">
+        <is>
+          <t>COmentario Imagen 1 PInterest</t>
+        </is>
+      </c>
+    </row>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204">
+      <c r="A204" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B204" s="33" t="inlineStr">
+        <is>
+          <t>Imagen Prueba Pinterest 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231">
+      <c r="A231" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B231" s="3" t="inlineStr">
+        <is>
+          <t>Comentario</t>
+        </is>
+      </c>
+    </row>
+    <row r="232"/>
+    <row r="233">
+      <c r="A233" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B233" s="0" t="inlineStr">
+        <is>
+          <t>Comentario Imagen Prueba Pinterest 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0" left="0" bottom="0" top="0" footer="0.5" header="0.5"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>